<commit_message>
supprimer seulement un span
</commit_message>
<xml_diff>
--- a/doc/scrum.xlsx
+++ b/doc/scrum.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="12330"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="12330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>Backlog</t>
   </si>
@@ -205,6 +205,18 @@
   </si>
   <si>
     <t>1/2 ok</t>
+  </si>
+  <si>
+    <t>TRUC à FAIRE NICOLAS</t>
+  </si>
+  <si>
+    <t>les tags</t>
+  </si>
+  <si>
+    <t>l'autompletion</t>
+  </si>
+  <si>
+    <t>trie des images</t>
   </si>
 </sst>
 </file>
@@ -603,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
@@ -1155,12 +1167,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>